<commit_message>
Added all friends view with filter.
</commit_message>
<xml_diff>
--- a/JS-Frameworks-Self-Evaluation-Protocol.xlsx
+++ b/JS-Frameworks-Self-Evaluation-Protocol.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\P. Ivanov\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\P. Ivanov\Documents\WebstormProjects\SocialNetwork-JS-Frameworks\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -657,8 +657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -732,7 +732,9 @@
       <c r="B8" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="6"/>
+      <c r="C8" s="6">
+        <v>9</v>
+      </c>
       <c r="D8" s="12" t="s">
         <v>18</v>
       </c>
@@ -742,7 +744,9 @@
       <c r="B9" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="6"/>
+      <c r="C9" s="6">
+        <v>16</v>
+      </c>
       <c r="D9" s="12" t="s">
         <v>18</v>
       </c>
@@ -856,7 +860,9 @@
       <c r="B19" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="5"/>
+      <c r="C19" s="5">
+        <v>10</v>
+      </c>
       <c r="D19" s="5">
         <v>10</v>
       </c>
@@ -1126,7 +1132,7 @@
       </c>
       <c r="C44" s="11">
         <f>SUM(C6:C43)</f>
-        <v>148</v>
+        <v>183</v>
       </c>
       <c r="D44" s="11">
         <v>370</v>

</xml_diff>